<commit_message>
Tablas En proceso de llenado
</commit_message>
<xml_diff>
--- a/docs/Datos.xlsx
+++ b/docs/Datos.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maria\Dropbox (Personal)\Universidad\Infracomp\Casos\Infracomp\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jd.torres11\Documents\GitHub\InfraComp\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4455" tabRatio="790"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4455" tabRatio="790" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Carga 400 - 1 thread" sheetId="1" r:id="rId1"/>
@@ -106,12 +106,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -141,10 +153,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -459,10 +479,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A2:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -474,37 +494,39 @@
     <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="5"/>
+      <c r="B2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B1">
+      <c r="C2" s="6">
         <v>400</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E2" s="6" t="s">
         <v>6</v>
       </c>
+      <c r="F2" s="5"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="B3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" s="1" t="s">
+      <c r="E3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>2</v>
       </c>
       <c r="H3" t="s">
@@ -518,10 +540,18 @@
       <c r="B4" s="1">
         <v>1</v>
       </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
+      <c r="C4" s="1">
+        <v>96516</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1">
+        <v>3201</v>
+      </c>
       <c r="H4" t="s">
         <v>9</v>
       </c>
@@ -533,10 +563,18 @@
       <c r="B5" s="1">
         <v>1</v>
       </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
+      <c r="C5" s="1">
+        <v>104419</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1">
+        <v>1695</v>
+      </c>
       <c r="H5" t="s">
         <v>10</v>
       </c>
@@ -548,10 +586,18 @@
       <c r="B6" s="1">
         <v>1</v>
       </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
+      <c r="C6" s="1">
+        <v>94912</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0</v>
+      </c>
+      <c r="F6" s="1">
+        <v>2278</v>
+      </c>
       <c r="H6" t="s">
         <v>11</v>
       </c>
@@ -563,10 +609,18 @@
       <c r="B7" s="1">
         <v>1</v>
       </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
+      <c r="C7" s="1">
+        <v>106473</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1">
+        <v>6301</v>
+      </c>
       <c r="H7" t="s">
         <v>12</v>
       </c>
@@ -578,10 +632,18 @@
       <c r="B8" s="1">
         <v>1</v>
       </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
+      <c r="C8" s="1">
+        <v>100980</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1">
+        <v>1</v>
+      </c>
+      <c r="F8" s="1">
+        <v>5163</v>
+      </c>
       <c r="H8" t="s">
         <v>13</v>
       </c>
@@ -593,10 +655,18 @@
       <c r="B9" s="1">
         <v>1</v>
       </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="2"/>
+      <c r="C9" s="1">
+        <v>100845</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0</v>
+      </c>
+      <c r="F9" s="2">
+        <v>4325</v>
+      </c>
       <c r="H9" t="s">
         <v>14</v>
       </c>
@@ -608,10 +678,18 @@
       <c r="B10" s="1">
         <v>1</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
+      <c r="C10" s="1">
+        <v>92478</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0</v>
+      </c>
+      <c r="F10" s="1">
+        <v>4041</v>
+      </c>
       <c r="H10" t="s">
         <v>15</v>
       </c>
@@ -623,10 +701,18 @@
       <c r="B11" s="1">
         <v>1</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
+      <c r="C11" s="1">
+        <v>101479</v>
+      </c>
+      <c r="D11" s="1">
+        <v>2</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0</v>
+      </c>
+      <c r="F11" s="1">
+        <v>2526</v>
+      </c>
       <c r="H11" t="s">
         <v>14</v>
       </c>
@@ -666,7 +752,7 @@
   <dimension ref="A4:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:D14"/>
+      <selection activeCell="A4" sqref="A4:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -674,26 +760,28 @@
     <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="B4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F4" s="1" t="s">
+      <c r="E4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>2</v>
       </c>
     </row>
@@ -704,10 +792,18 @@
       <c r="B5" s="1">
         <v>2</v>
       </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
+      <c r="C5" s="1">
+        <v>55005</v>
+      </c>
+      <c r="D5" s="1">
+        <v>2</v>
+      </c>
+      <c r="E5" s="1">
+        <v>4</v>
+      </c>
+      <c r="F5" s="1">
+        <v>4506</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
@@ -716,10 +812,18 @@
       <c r="B6" s="1">
         <v>2</v>
       </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
+      <c r="C6" s="1">
+        <v>47176</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0</v>
+      </c>
+      <c r="F6" s="1">
+        <v>3427</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
@@ -728,10 +832,18 @@
       <c r="B7" s="1">
         <v>2</v>
       </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
+      <c r="C7" s="1">
+        <v>50656</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1">
+        <v>1</v>
+      </c>
+      <c r="F7" s="1">
+        <v>4775</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
@@ -740,10 +852,18 @@
       <c r="B8" s="1">
         <v>2</v>
       </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
+      <c r="C8" s="1">
+        <v>48553</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0</v>
+      </c>
+      <c r="F8" s="1">
+        <v>3402</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
@@ -752,10 +872,18 @@
       <c r="B9" s="1">
         <v>2</v>
       </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
+      <c r="C9" s="1">
+        <v>49723</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1">
+        <v>1</v>
+      </c>
+      <c r="F9" s="1">
+        <v>5056</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
@@ -764,10 +892,18 @@
       <c r="B10" s="1">
         <v>2</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="2"/>
+      <c r="C10" s="1">
+        <v>47329</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1">
+        <v>1</v>
+      </c>
+      <c r="F10" s="2">
+        <v>5277</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
@@ -776,10 +912,18 @@
       <c r="B11" s="1">
         <v>2</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
+      <c r="C11" s="1">
+        <v>48466</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0</v>
+      </c>
+      <c r="F11" s="1">
+        <v>6003</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
@@ -788,10 +932,18 @@
       <c r="B12" s="1">
         <v>2</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
+      <c r="C12" s="1">
+        <v>48953</v>
+      </c>
+      <c r="D12" s="1">
+        <v>1</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0</v>
+      </c>
+      <c r="F12" s="1">
+        <v>3698</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
@@ -827,7 +979,7 @@
   <dimension ref="G4:L14"/>
   <sheetViews>
     <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4:J14"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -835,26 +987,27 @@
     <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="24.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="I4" s="1" t="s">
+      <c r="H4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="J4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="K4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="L4" s="1" t="s">
+      <c r="K4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L4" s="3" t="s">
         <v>2</v>
       </c>
     </row>
@@ -865,10 +1018,18 @@
       <c r="H5" s="1">
         <v>8</v>
       </c>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
+      <c r="I5" s="1">
+        <v>24619</v>
+      </c>
+      <c r="J5" s="1">
+        <v>7</v>
+      </c>
+      <c r="K5" s="1">
+        <v>0</v>
+      </c>
+      <c r="L5" s="1">
+        <v>13625</v>
+      </c>
     </row>
     <row r="6" spans="7:12" x14ac:dyDescent="0.25">
       <c r="G6" s="1">
@@ -877,10 +1038,18 @@
       <c r="H6" s="1">
         <v>8</v>
       </c>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
+      <c r="I6" s="1">
+        <v>24135</v>
+      </c>
+      <c r="J6" s="1">
+        <v>4</v>
+      </c>
+      <c r="K6" s="1">
+        <v>1</v>
+      </c>
+      <c r="L6" s="1">
+        <v>5748</v>
+      </c>
     </row>
     <row r="7" spans="7:12" x14ac:dyDescent="0.25">
       <c r="G7" s="1">
@@ -889,10 +1058,18 @@
       <c r="H7" s="1">
         <v>8</v>
       </c>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
+      <c r="I7" s="1">
+        <v>24460</v>
+      </c>
+      <c r="J7" s="1">
+        <v>3</v>
+      </c>
+      <c r="K7" s="1">
+        <v>0</v>
+      </c>
+      <c r="L7" s="1">
+        <v>6470</v>
+      </c>
     </row>
     <row r="8" spans="7:12" x14ac:dyDescent="0.25">
       <c r="G8" s="1">
@@ -901,10 +1078,18 @@
       <c r="H8" s="1">
         <v>8</v>
       </c>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
+      <c r="I8" s="1">
+        <v>22388</v>
+      </c>
+      <c r="J8" s="1">
+        <v>5</v>
+      </c>
+      <c r="K8" s="1">
+        <v>0</v>
+      </c>
+      <c r="L8" s="1">
+        <v>4695</v>
+      </c>
     </row>
     <row r="9" spans="7:12" x14ac:dyDescent="0.25">
       <c r="G9" s="1">
@@ -913,10 +1098,18 @@
       <c r="H9" s="1">
         <v>8</v>
       </c>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
+      <c r="I9" s="1">
+        <v>23256</v>
+      </c>
+      <c r="J9" s="1">
+        <v>3</v>
+      </c>
+      <c r="K9" s="1">
+        <v>0</v>
+      </c>
+      <c r="L9" s="1">
+        <v>8649</v>
+      </c>
     </row>
     <row r="10" spans="7:12" x14ac:dyDescent="0.25">
       <c r="G10" s="1">
@@ -925,10 +1118,18 @@
       <c r="H10" s="1">
         <v>8</v>
       </c>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="2"/>
+      <c r="I10" s="1">
+        <v>22680</v>
+      </c>
+      <c r="J10" s="1">
+        <v>2</v>
+      </c>
+      <c r="K10" s="1">
+        <v>0</v>
+      </c>
+      <c r="L10" s="2">
+        <v>14689</v>
+      </c>
     </row>
     <row r="11" spans="7:12" x14ac:dyDescent="0.25">
       <c r="G11" s="1">
@@ -937,10 +1138,18 @@
       <c r="H11" s="1">
         <v>8</v>
       </c>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
+      <c r="I11" s="1">
+        <v>22309</v>
+      </c>
+      <c r="J11" s="1">
+        <v>3</v>
+      </c>
+      <c r="K11" s="1">
+        <v>0</v>
+      </c>
+      <c r="L11" s="1">
+        <v>6539</v>
+      </c>
     </row>
     <row r="12" spans="7:12" x14ac:dyDescent="0.25">
       <c r="G12" s="1">
@@ -949,10 +1158,18 @@
       <c r="H12" s="1">
         <v>8</v>
       </c>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
+      <c r="I12" s="1">
+        <v>21242</v>
+      </c>
+      <c r="J12" s="1">
+        <v>2</v>
+      </c>
+      <c r="K12" s="1">
+        <v>1</v>
+      </c>
+      <c r="L12" s="1">
+        <v>16923</v>
+      </c>
     </row>
     <row r="13" spans="7:12" x14ac:dyDescent="0.25">
       <c r="G13" s="1">
@@ -985,10 +1202,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A3:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -997,40 +1214,43 @@
     <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1">
+      <c r="C3" s="4">
         <v>200</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D1">
+      <c r="E3" s="4">
         <v>40</v>
       </c>
+      <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="B4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F4" s="1" t="s">
+      <c r="E4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1041,10 +1261,18 @@
       <c r="B5" s="1">
         <v>1</v>
       </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
+      <c r="C5" s="1">
+        <v>48498</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1">
+        <v>2709</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
@@ -1053,10 +1281,18 @@
       <c r="B6" s="1">
         <v>1</v>
       </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
+      <c r="C6" s="1">
+        <v>56538</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0</v>
+      </c>
+      <c r="F6" s="1">
+        <v>4487</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
@@ -1065,10 +1301,18 @@
       <c r="B7" s="1">
         <v>1</v>
       </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
+      <c r="C7" s="1">
+        <v>51537</v>
+      </c>
+      <c r="D7" s="1">
+        <v>4</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1">
+        <v>3969</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
@@ -1077,10 +1321,18 @@
       <c r="B8" s="1">
         <v>1</v>
       </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
+      <c r="C8" s="1">
+        <v>65643</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1">
+        <v>2</v>
+      </c>
+      <c r="F8" s="1">
+        <v>5114</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
@@ -1089,10 +1341,18 @@
       <c r="B9" s="1">
         <v>1</v>
       </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
+      <c r="C9" s="1">
+        <v>46764</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0</v>
+      </c>
+      <c r="F9" s="1">
+        <v>3318</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
@@ -1101,10 +1361,18 @@
       <c r="B10" s="1">
         <v>1</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="2"/>
+      <c r="C10" s="1">
+        <v>50434</v>
+      </c>
+      <c r="D10" s="1">
+        <v>1</v>
+      </c>
+      <c r="E10" s="1">
+        <v>1</v>
+      </c>
+      <c r="F10" s="2">
+        <v>3539</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
@@ -1113,10 +1381,18 @@
       <c r="B11" s="1">
         <v>1</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
+      <c r="C11" s="1">
+        <v>48355</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0</v>
+      </c>
+      <c r="F11" s="1">
+        <v>2665</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
@@ -1125,10 +1401,18 @@
       <c r="B12" s="1">
         <v>1</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
+      <c r="C12" s="1">
+        <v>41581</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0</v>
+      </c>
+      <c r="F12" s="1">
+        <v>3509</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
@@ -1163,8 +1447,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>